<commit_message>
Changed timetable for 6 students and added the tasks
</commit_message>
<xml_diff>
--- a/Things we have to hand in weekly/Sprint planning.xlsx
+++ b/Things we have to hand in weekly/Sprint planning.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\20181903\Documents\GitHub\DBLVis\Things we have to hand in weekly\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\20181751\OneDrive - TU Eindhoven\Documents\GitHub\DBLVis\Things we have to hand in weekly\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{63E0F895-0B47-4B9C-9E88-435C586C2823}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5A99C1D-3DBF-4FD5-BDCD-D2AC94D13EBB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" xr2:uid="{7CBC9F4E-9AFF-44EB-9A30-048360895DCE}"/>
   </bookViews>
@@ -565,10 +565,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73B6C823-4AFD-4954-9F30-B738F1F450FA}">
-  <dimension ref="A1:F28"/>
+  <dimension ref="A1:F26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G34" sqref="G34"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -719,175 +719,183 @@
       </c>
       <c r="E11" s="2"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A12" s="2"/>
-      <c r="B12" s="2"/>
-      <c r="C12" s="2"/>
-      <c r="D12" s="2"/>
-      <c r="E12" s="2"/>
-    </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A13" s="2"/>
-      <c r="B13" s="2"/>
-      <c r="C13" s="2"/>
-      <c r="D13" s="2"/>
-      <c r="E13" s="2"/>
+      <c r="A13" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A14" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A15" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="F15" s="3" t="s">
-        <v>41</v>
+      <c r="A15" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>28</v>
-      </c>
+        <v>3</v>
+      </c>
+      <c r="B16" s="2"/>
       <c r="C16" s="2" t="s">
-        <v>42</v>
+        <v>14</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A17" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>29</v>
-      </c>
+      <c r="A17" s="2"/>
+      <c r="B17" s="2"/>
       <c r="C17" s="2" t="s">
-        <v>13</v>
+        <v>43</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>8</v>
+        <v>19</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A18" s="2" t="s">
-        <v>3</v>
-      </c>
+      <c r="A18" s="2"/>
       <c r="B18" s="2"/>
       <c r="C18" s="2" t="s">
-        <v>14</v>
+        <v>44</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" s="2"/>
       <c r="B19" s="2"/>
       <c r="C19" s="2" t="s">
-        <v>43</v>
+        <v>15</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" s="2"/>
       <c r="B20" s="2"/>
       <c r="C20" s="2" t="s">
-        <v>44</v>
+        <v>16</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" s="2"/>
       <c r="B21" s="2"/>
       <c r="C21" s="2" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="D21" s="2" t="s">
         <v>10</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" s="2"/>
       <c r="B22" s="2"/>
       <c r="C22" s="2" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" s="2"/>
       <c r="B23" s="2"/>
       <c r="C23" s="2" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="D23" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E23" s="2" t="s">
-        <v>38</v>
-      </c>
+      <c r="E23" s="2"/>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" s="2"/>
       <c r="B24" s="2"/>
       <c r="C24" s="2" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="D24" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E24" s="2" t="s">
-        <v>39</v>
-      </c>
+      <c r="E24" s="2"/>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" s="2"/>
       <c r="B25" s="2"/>
       <c r="C25" s="2" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>10</v>
+        <v>24</v>
       </c>
       <c r="E25" s="2"/>
     </row>
@@ -895,34 +903,12 @@
       <c r="A26" s="2"/>
       <c r="B26" s="2"/>
       <c r="C26" s="2" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="E26" s="2"/>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A27" s="2"/>
-      <c r="B27" s="2"/>
-      <c r="C27" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="D27" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="E27" s="2"/>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A28" s="2"/>
-      <c r="B28" s="2"/>
-      <c r="C28" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="D28" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E28" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>